<commit_message>
Readme updated, COM automaticly detected
</commit_message>
<xml_diff>
--- a/resources/actions/stimuli/practice.xlsx
+++ b/resources/actions/stimuli/practice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Desktop\CNC\Paradigmas\Python\Rutvik\picture-plausability\resources\actions\stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\OneDrive\Desktop\CNC\Paradigmas\Python\Rutvik\rutvik-picture-plausability\resources\actions\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D609FE-9F57-4ED0-B97E-67E15B95DEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90853816-A519-408A-8573-B3B971653235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1631BE85-4D3D-4F09-8AE2-3287BF9C0372}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1631BE85-4D3D-4F09-8AE2-3287BF9C0372}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,24 +41,15 @@
     <t>plausible</t>
   </si>
   <si>
-    <t>j</t>
-  </si>
-  <si>
     <t>bathing</t>
   </si>
   <si>
-    <t>bañándose</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
     <t>buttoning</t>
   </si>
   <si>
-    <t>abotonándose</t>
-  </si>
-  <si>
     <t>implaus</t>
   </si>
   <si>
@@ -68,9 +59,6 @@
     <t>na</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
     <t>x25</t>
   </si>
   <si>
@@ -105,6 +93,18 @@
   </si>
   <si>
     <t>resources/pictures/swimGrass.png</t>
+  </si>
+  <si>
+    <t>bañarse</t>
+  </si>
+  <si>
+    <t>abotonar</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
   </si>
 </sst>
 </file>
@@ -508,37 +508,38 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.77734375" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -549,19 +550,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -569,59 +570,59 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>